<commit_message>
laver priser og så videre
</commit_message>
<xml_diff>
--- a/Estimering/loebpriser.xlsx
+++ b/Estimering/loebpriser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasmuskaslund/Documents/GitHub/SpecialeJR /Estimering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5BA477-D7AE-3C4C-BDE7-25D471ACA86B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BBA687-7D43-A84B-923C-EBF92F3AA059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="94">
   <si>
     <t>1994</t>
   </si>
@@ -304,12 +304,21 @@
   <si>
     <t>Egen_gruppe</t>
   </si>
+  <si>
+    <t>Indkomstgruppe</t>
+  </si>
+  <si>
+    <t>Gennemsnitshustand</t>
+  </si>
+  <si>
+    <t>Under 250.000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -320,6 +329,11 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -655,12 +669,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC283"/>
+  <dimension ref="A1:AD283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A11" sqref="A11"/>
-      <selection pane="topRight" activeCell="AB1" sqref="AB1:AC283"/>
+      <selection pane="topRight" activeCell="AE57" sqref="AE57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -669,7 +683,7 @@
     <col min="2" max="27" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -757,8 +771,11 @@
       <c r="AC1" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -846,8 +863,11 @@
       <c r="AC2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -935,8 +955,11 @@
       <c r="AC3" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1024,8 +1047,11 @@
       <c r="AC4" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1113,8 +1139,11 @@
       <c r="AC5" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1202,8 +1231,11 @@
       <c r="AC6" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -1291,8 +1323,11 @@
       <c r="AC7" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1380,8 +1415,11 @@
       <c r="AC8" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1469,8 +1507,11 @@
       <c r="AC9" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1558,8 +1599,11 @@
       <c r="AC10" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1647,8 +1691,11 @@
       <c r="AC11" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1736,8 +1783,11 @@
       <c r="AC12" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1825,8 +1875,11 @@
       <c r="AC13" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1914,8 +1967,11 @@
       <c r="AC14" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -2003,8 +2059,11 @@
       <c r="AC15" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -2092,8 +2151,11 @@
       <c r="AC16" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -2181,8 +2243,11 @@
       <c r="AC17" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2270,8 +2335,11 @@
       <c r="AC18" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -2359,8 +2427,11 @@
       <c r="AC19" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -2448,8 +2519,11 @@
       <c r="AC20" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -2537,8 +2611,11 @@
       <c r="AC21" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -2626,8 +2703,11 @@
       <c r="AC22" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
@@ -2715,8 +2795,11 @@
       <c r="AC23" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -2804,8 +2887,11 @@
       <c r="AC24" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -2893,8 +2979,11 @@
       <c r="AC25" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -2982,8 +3071,11 @@
       <c r="AC26" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -3071,8 +3163,11 @@
       <c r="AC27" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -3160,8 +3255,11 @@
       <c r="AC28" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
@@ -3249,8 +3347,11 @@
       <c r="AC29" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -3338,8 +3439,11 @@
       <c r="AC30" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
@@ -3427,8 +3531,11 @@
       <c r="AC31" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
@@ -3516,8 +3623,11 @@
       <c r="AC32" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
@@ -3605,8 +3715,11 @@
       <c r="AC33" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
@@ -3694,8 +3807,11 @@
       <c r="AC34" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -3783,8 +3899,11 @@
       <c r="AC35" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>59</v>
       </c>
@@ -3872,8 +3991,11 @@
       <c r="AC36" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -3961,8 +4083,11 @@
       <c r="AC37" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>61</v>
       </c>
@@ -4050,8 +4175,11 @@
       <c r="AC38" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>62</v>
       </c>
@@ -4139,8 +4267,11 @@
       <c r="AC39" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
@@ -4228,8 +4359,11 @@
       <c r="AC40" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -4317,8 +4451,11 @@
       <c r="AC41" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -4406,8 +4543,11 @@
       <c r="AC42" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>66</v>
       </c>
@@ -4495,8 +4635,11 @@
       <c r="AC43" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>67</v>
       </c>
@@ -4584,8 +4727,11 @@
       <c r="AC44" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
@@ -4673,8 +4819,11 @@
       <c r="AC45" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>69</v>
       </c>
@@ -4762,8 +4911,11 @@
       <c r="AC46" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>70</v>
       </c>
@@ -4851,8 +5003,11 @@
       <c r="AC47" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>71</v>
       </c>
@@ -4940,8 +5095,11 @@
       <c r="AC48" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>74</v>
       </c>
@@ -5029,8 +5187,11 @@
       <c r="AC49" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
@@ -5118,8 +5279,11 @@
       <c r="AC50" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -5208,7 +5372,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>28</v>
       </c>
@@ -5297,7 +5461,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>29</v>
       </c>
@@ -5386,7 +5550,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
@@ -5475,7 +5639,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>31</v>
       </c>
@@ -5564,7 +5728,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>32</v>
       </c>
@@ -5653,7 +5817,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>33</v>
       </c>
@@ -5742,7 +5906,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
@@ -5831,7 +5995,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
@@ -5920,7 +6084,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>36</v>
       </c>
@@ -6009,7 +6173,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>37</v>
       </c>
@@ -6098,7 +6262,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>38</v>
       </c>
@@ -6187,7 +6351,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>39</v>
       </c>
@@ -6276,7 +6440,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
@@ -25857,6 +26021,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>